<commit_message>
added steel demand getter funcion
</commit_message>
<xml_diff>
--- a/import_data/Feedstock Prices.xlsx
+++ b/import_data/Feedstock Prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{8A860862-830F-487D-AF1E-50CDDEEF4A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE89D81B-CB1E-40BC-ACA2-7648B9E42133}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{8A860862-830F-487D-AF1E-50CDDEEF4A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4918A6-F5B0-45F7-B20A-C1DE8069A7F1}"/>
   <bookViews>
-    <workbookView xWindow="1047" yWindow="1047" windowWidth="19200" windowHeight="9613" xr2:uid="{28E9977C-84A3-43AD-AF96-4E089B66DB2E}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{28E9977C-84A3-43AD-AF96-4E089B66DB2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>EUR / t</t>
+  </si>
+  <si>
+    <t>EUR / kg</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -533,6 +539,9 @@
         <f>97.73*0.877</f>
         <v>85.709209999999999</v>
       </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,6 +563,9 @@
         <f>224.46*0.877</f>
         <v>196.85142000000002</v>
       </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
@@ -575,6 +587,9 @@
         <f>300.67*0.877</f>
         <v>263.68759</v>
       </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -596,6 +611,9 @@
         <f>121.86*0.877</f>
         <v>106.87121999999999</v>
       </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
@@ -617,6 +635,9 @@
         <f>-27.5*0.877/1000</f>
         <v>-2.41175E-2</v>
       </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
@@ -636,6 +657,9 @@
       </c>
       <c r="D7">
         <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -662,12 +686,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -836,15 +857,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA233994-C021-4EE2-891B-792745C54C2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44FEDDF4-819D-45CF-9D9D-71A79C44C95F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -869,18 +902,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44FEDDF4-819D-45CF-9D9D-71A79C44C95F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA233994-C021-4EE2-891B-792745C54C2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>